<commit_message>
With held reconcilation fee
</commit_message>
<xml_diff>
--- a/Demo_working/Tax1099Automation-master/Demo_working/src/test/resources/TestData/TestData.xlsx
+++ b/Demo_working/Tax1099Automation-master/Demo_working/src/test/resources/TestData/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2472" windowWidth="17220" windowHeight="4296" tabRatio="706" firstSheet="11" activeTab="15"/>
+    <workbookView xWindow="0" yWindow="2472" windowWidth="16920" windowHeight="8220" tabRatio="706" firstSheet="11" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -26,12 +26,12 @@
     <sheet name="StateID-Validations" sheetId="18" r:id="rId17"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A4:I17"/>
+  <oleSize ref="A1:I27"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="212">
   <si>
     <t>TestCases</t>
   </si>
@@ -503,15 +503,6 @@
     <t>Should have 7 digits,hyphen and 2 Alphabets</t>
   </si>
   <si>
-    <t>Test03052021124952</t>
-  </si>
-  <si>
-    <t>51-3476967</t>
-  </si>
-  <si>
-    <t>Test03052021125559</t>
-  </si>
-  <si>
     <t>Reconsillation details</t>
   </si>
   <si>
@@ -524,31 +515,163 @@
     <t>Status</t>
   </si>
   <si>
-    <t>Test0305202172125</t>
-  </si>
-  <si>
-    <t>25-3597885</t>
-  </si>
-  <si>
-    <t>Test0305202172737</t>
-  </si>
-  <si>
-    <t>Test0305202174902</t>
-  </si>
-  <si>
-    <t>79-7546968</t>
-  </si>
-  <si>
-    <t>Test0305202175512</t>
-  </si>
-  <si>
-    <t>Test0305202183207</t>
-  </si>
-  <si>
-    <t>80-1825910</t>
-  </si>
-  <si>
-    <t>Test0305202183817</t>
+    <t>Test03082021111834</t>
+  </si>
+  <si>
+    <t>22-7415820</t>
+  </si>
+  <si>
+    <t>Test03082021112444</t>
+  </si>
+  <si>
+    <t>Test0308202172425</t>
+  </si>
+  <si>
+    <t>78-388821_</t>
+  </si>
+  <si>
+    <t>Test0308202173136</t>
+  </si>
+  <si>
+    <t>Test0308202174907</t>
+  </si>
+  <si>
+    <t>Test0308202183215</t>
+  </si>
+  <si>
+    <t>35010-</t>
+  </si>
+  <si>
+    <t>92-2793200</t>
+  </si>
+  <si>
+    <t>Test0308202184002</t>
+  </si>
+  <si>
+    <t>03/15/2021</t>
+  </si>
+  <si>
+    <t>201204734</t>
+  </si>
+  <si>
+    <t>Test0309202195319</t>
+  </si>
+  <si>
+    <t>41-0350344</t>
+  </si>
+  <si>
+    <t>Test0309202195928</t>
+  </si>
+  <si>
+    <t>201204735</t>
+  </si>
+  <si>
+    <t>Test03092021113259</t>
+  </si>
+  <si>
+    <t>75-9272649</t>
+  </si>
+  <si>
+    <t>Test03092021113908</t>
+  </si>
+  <si>
+    <t>Test0309202163649</t>
+  </si>
+  <si>
+    <t>87-9197398</t>
+  </si>
+  <si>
+    <t>Test0309202164307</t>
+  </si>
+  <si>
+    <t>Test0309202170229</t>
+  </si>
+  <si>
+    <t>22-6736069</t>
+  </si>
+  <si>
+    <t>Test0309202170839</t>
+  </si>
+  <si>
+    <t>201204738</t>
+  </si>
+  <si>
+    <t>Test0309202173317</t>
+  </si>
+  <si>
+    <t>61-6703041</t>
+  </si>
+  <si>
+    <t>Test0309202173927</t>
+  </si>
+  <si>
+    <t>201204739</t>
+  </si>
+  <si>
+    <t>Test0309202180316</t>
+  </si>
+  <si>
+    <t>70-1315274</t>
+  </si>
+  <si>
+    <t>Test0309202180928</t>
+  </si>
+  <si>
+    <t>201204740</t>
+  </si>
+  <si>
+    <t>Test03102021102015</t>
+  </si>
+  <si>
+    <t>87-5903288</t>
+  </si>
+  <si>
+    <t>Test03102021102627</t>
+  </si>
+  <si>
+    <t>201204744</t>
+  </si>
+  <si>
+    <t>Test03102021112930</t>
+  </si>
+  <si>
+    <t>30-0946773</t>
+  </si>
+  <si>
+    <t>Test03102021113540</t>
+  </si>
+  <si>
+    <t>Test03102021121907</t>
+  </si>
+  <si>
+    <t>45-1244425</t>
+  </si>
+  <si>
+    <t>Test03102021122517</t>
+  </si>
+  <si>
+    <t>Test0310202154628</t>
+  </si>
+  <si>
+    <t>96-5189304</t>
+  </si>
+  <si>
+    <t>Test0310202155236</t>
+  </si>
+  <si>
+    <t>201204747</t>
+  </si>
+  <si>
+    <t>Test0310202165232</t>
+  </si>
+  <si>
+    <t>96-8531926</t>
+  </si>
+  <si>
+    <t>Test0310202165905</t>
+  </si>
+  <si>
+    <t>201204749</t>
   </si>
 </sst>
 </file>
@@ -1406,9 +1529,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
@@ -1626,8 +1747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1655,7 +1776,7 @@
         <v>123</v>
       </c>
       <c r="B3" t="s">
-        <v>170</v>
+        <v>210</v>
       </c>
     </row>
     <row r="4">
@@ -1663,23 +1784,23 @@
         <v>140</v>
       </c>
       <c r="B4" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="5">
       <c r="A5" t="s">
         <v>120</v>
       </c>
       <c r="B5" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="12" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
         <v>121</v>
       </c>
-      <c r="B8" s="12" t="s">
-        <v>139</v>
+      <c r="B8" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="9">
@@ -1687,7 +1808,7 @@
         <v>122</v>
       </c>
       <c r="B9" t="s">
-        <v>169</v>
+        <v>209</v>
       </c>
     </row>
     <row r="10">
@@ -1735,7 +1856,7 @@
         <v>133</v>
       </c>
       <c r="B16" t="n">
-        <v>2.36894931E8</v>
+        <v>1.62021761E8</v>
       </c>
     </row>
     <row r="17">
@@ -1772,22 +1893,22 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="12" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="12" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="12" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="12" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Test case 5 edit with held amount
</commit_message>
<xml_diff>
--- a/Demo_working/Tax1099Automation-master/Demo_working/src/test/resources/TestData/TestData.xlsx
+++ b/Demo_working/Tax1099Automation-master/Demo_working/src/test/resources/TestData/TestData.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1016" uniqueCount="270">
   <si>
     <t>TestCases</t>
   </si>
@@ -672,6 +672,180 @@
   </si>
   <si>
     <t>201204749</t>
+  </si>
+  <si>
+    <t>Test03112021122222</t>
+  </si>
+  <si>
+    <t>46-6261343</t>
+  </si>
+  <si>
+    <t>Test03112021122831</t>
+  </si>
+  <si>
+    <t>201204760</t>
+  </si>
+  <si>
+    <t>Test0311202143558</t>
+  </si>
+  <si>
+    <t>96-524994_</t>
+  </si>
+  <si>
+    <t>Test0311202144205</t>
+  </si>
+  <si>
+    <t>Test0311202145327</t>
+  </si>
+  <si>
+    <t>38-3766247</t>
+  </si>
+  <si>
+    <t>Test0311202145932</t>
+  </si>
+  <si>
+    <t>201204762</t>
+  </si>
+  <si>
+    <t>Test0311202154827</t>
+  </si>
+  <si>
+    <t>49-4920679</t>
+  </si>
+  <si>
+    <t>Test0311202155436</t>
+  </si>
+  <si>
+    <t>201204763</t>
+  </si>
+  <si>
+    <t>Test03122021112932</t>
+  </si>
+  <si>
+    <t>97-2080956</t>
+  </si>
+  <si>
+    <t>Test03122021113542</t>
+  </si>
+  <si>
+    <t>201204773</t>
+  </si>
+  <si>
+    <t>Test0312202111102</t>
+  </si>
+  <si>
+    <t>Test0312202114015</t>
+  </si>
+  <si>
+    <t>75-5790047</t>
+  </si>
+  <si>
+    <t>Test0312202114626</t>
+  </si>
+  <si>
+    <t>201204774</t>
+  </si>
+  <si>
+    <t>Test0312202125315</t>
+  </si>
+  <si>
+    <t>53-0701817</t>
+  </si>
+  <si>
+    <t>Test0312202125924</t>
+  </si>
+  <si>
+    <t>Test0312202135521</t>
+  </si>
+  <si>
+    <t>69-7341572</t>
+  </si>
+  <si>
+    <t>Test0312202140129</t>
+  </si>
+  <si>
+    <t>201204775</t>
+  </si>
+  <si>
+    <t>Test0312202145645</t>
+  </si>
+  <si>
+    <t>38-5681801</t>
+  </si>
+  <si>
+    <t>Test0312202150254</t>
+  </si>
+  <si>
+    <t>201204776</t>
+  </si>
+  <si>
+    <t>Test0312202153149</t>
+  </si>
+  <si>
+    <t>38-2832699</t>
+  </si>
+  <si>
+    <t>Test0312202153800</t>
+  </si>
+  <si>
+    <t>201204777</t>
+  </si>
+  <si>
+    <t>Test0312202162542</t>
+  </si>
+  <si>
+    <t>25-0761030</t>
+  </si>
+  <si>
+    <t>Test0312202163153</t>
+  </si>
+  <si>
+    <t>201204778</t>
+  </si>
+  <si>
+    <t>Test0312202170743</t>
+  </si>
+  <si>
+    <t>52-8498274</t>
+  </si>
+  <si>
+    <t>Test0312202171351</t>
+  </si>
+  <si>
+    <t>Test0312202173211</t>
+  </si>
+  <si>
+    <t>38-1799939</t>
+  </si>
+  <si>
+    <t>Test0312202173822</t>
+  </si>
+  <si>
+    <t>201204779</t>
+  </si>
+  <si>
+    <t>Test0312202181514</t>
+  </si>
+  <si>
+    <t>35-2956088</t>
+  </si>
+  <si>
+    <t>Test0312202182121</t>
+  </si>
+  <si>
+    <t>201204780</t>
+  </si>
+  <si>
+    <t>Test0312202190806</t>
+  </si>
+  <si>
+    <t>74-2042568</t>
+  </si>
+  <si>
+    <t>Test0312202191417</t>
+  </si>
+  <si>
+    <t>201204782</t>
   </si>
 </sst>
 </file>
@@ -1776,7 +1950,7 @@
         <v>123</v>
       </c>
       <c r="B3" t="s">
-        <v>210</v>
+        <v>268</v>
       </c>
     </row>
     <row r="4">
@@ -1784,7 +1958,7 @@
         <v>140</v>
       </c>
       <c r="B4" t="s">
-        <v>208</v>
+        <v>266</v>
       </c>
     </row>
     <row r="5">
@@ -1792,7 +1966,7 @@
         <v>120</v>
       </c>
       <c r="B5" t="s">
-        <v>211</v>
+        <v>269</v>
       </c>
     </row>
     <row r="8">
@@ -1808,7 +1982,7 @@
         <v>122</v>
       </c>
       <c r="B9" t="s">
-        <v>209</v>
+        <v>267</v>
       </c>
     </row>
     <row r="10">
@@ -1856,7 +2030,7 @@
         <v>133</v>
       </c>
       <c r="B16" t="n">
-        <v>1.62021761E8</v>
+        <v>9.01864257E8</v>
       </c>
     </row>
     <row r="17">

</xml_diff>